<commit_message>
added folder & proj nodes for m monster
</commit_message>
<xml_diff>
--- a/src/VisualStudioMarketPlaceAssets/notes.xlsx
+++ b/src/VisualStudioMarketPlaceAssets/notes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="45">
   <si>
     <t>altova</t>
   </si>
@@ -164,6 +164,9 @@
   </si>
   <si>
     <t>not allowed</t>
+  </si>
+  <si>
+    <t>TODO ?</t>
   </si>
 </sst>
 </file>
@@ -223,7 +226,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -266,6 +269,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -279,7 +288,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -327,6 +336,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -612,7 +627,7 @@
   <dimension ref="A1:AI25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.25"/>
@@ -1197,10 +1212,10 @@
         <v>28</v>
       </c>
       <c r="F11" s="16" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="H11" s="13" t="s">
         <v>22</v>
@@ -1817,11 +1832,11 @@
       <c r="E23" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F23" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="G23" s="16" t="s">
-        <v>21</v>
+      <c r="F23" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="G23" s="18" t="s">
+        <v>30</v>
       </c>
       <c r="H23" s="13" t="s">
         <v>22</v>
@@ -1838,10 +1853,10 @@
       <c r="C24" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="D24" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E24" s="2" t="s">
+      <c r="D24" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="E24" s="17" t="s">
         <v>28</v>
       </c>
       <c r="F24" s="16" t="s">

</xml_diff>

<commit_message>
added proj & folder to xmlspy
</commit_message>
<xml_diff>
--- a/src/VisualStudioMarketPlaceAssets/notes.xlsx
+++ b/src/VisualStudioMarketPlaceAssets/notes.xlsx
@@ -226,7 +226,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -269,12 +269,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -288,7 +282,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -339,9 +333,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -627,7 +618,7 @@
   <dimension ref="A1:AI25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.25"/>
@@ -1832,10 +1823,10 @@
       <c r="E23" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F23" s="18" t="s">
+      <c r="F23" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G23" s="18" t="s">
+      <c r="G23" s="2" t="s">
         <v>30</v>
       </c>
       <c r="H23" s="13" t="s">

</xml_diff>

<commit_message>
add folder & proj node to emacs
</commit_message>
<xml_diff>
--- a/src/VisualStudioMarketPlaceAssets/notes.xlsx
+++ b/src/VisualStudioMarketPlaceAssets/notes.xlsx
@@ -618,7 +618,7 @@
   <dimension ref="A1:AI25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="F11" sqref="F11:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.25"/>
@@ -1202,11 +1202,11 @@
       <c r="E11" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="G11" s="16" t="s">
-        <v>44</v>
+      <c r="F11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="H11" s="13" t="s">
         <v>22</v>
@@ -1581,10 +1581,10 @@
         <v>28</v>
       </c>
       <c r="F18" s="16" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="G18" s="16" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="H18" s="13" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
add proj & folder node to vs2017 comm.
</commit_message>
<xml_diff>
--- a/src/VisualStudioMarketPlaceAssets/notes.xlsx
+++ b/src/VisualStudioMarketPlaceAssets/notes.xlsx
@@ -166,7 +166,7 @@
     <t>not allowed</t>
   </si>
   <si>
-    <t>TODO ?</t>
+    <t>TODO test at spur</t>
   </si>
 </sst>
 </file>
@@ -226,7 +226,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -269,6 +269,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -282,7 +294,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -332,7 +344,10 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -618,7 +633,7 @@
   <dimension ref="A1:AI25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11:G11"/>
+      <selection activeCell="F15" sqref="F15:G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.25"/>
@@ -1256,10 +1271,10 @@
       <c r="E12" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F12" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="G12" s="16" t="s">
+      <c r="F12" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="18" t="s">
         <v>21</v>
       </c>
       <c r="H12" s="13" t="s">
@@ -1310,10 +1325,10 @@
       <c r="E13" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F13" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="G13" s="16" t="s">
+      <c r="F13" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" s="18" t="s">
         <v>21</v>
       </c>
       <c r="H13" s="13" t="s">
@@ -1364,10 +1379,10 @@
       <c r="E14" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F14" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="G14" s="16" t="s">
+      <c r="F14" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" s="18" t="s">
         <v>21</v>
       </c>
       <c r="H14" s="13" t="s">
@@ -1418,11 +1433,11 @@
       <c r="E15" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F15" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="G15" s="16" t="s">
-        <v>21</v>
+      <c r="F15" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="G15" s="17" t="s">
+        <v>30</v>
       </c>
       <c r="H15" s="13" t="s">
         <v>21</v>
@@ -1472,10 +1487,10 @@
       <c r="E16" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F16" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="G16" s="16" t="s">
+      <c r="F16" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="G16" s="18" t="s">
         <v>21</v>
       </c>
       <c r="H16" s="13" t="s">
@@ -1526,10 +1541,10 @@
       <c r="E17" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F17" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="G17" s="16" t="s">
+      <c r="F17" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" s="18" t="s">
         <v>21</v>
       </c>
       <c r="H17" s="13" t="s">
@@ -1851,10 +1866,10 @@
         <v>28</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="G24" s="16" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="H24" s="13" t="s">
         <v>22</v>

</xml_diff>